<commit_message>
more notes, summary figure
</commit_message>
<xml_diff>
--- a/alignments/reports/pseudReports_blastBasedAlignments_2021_Jan13.xlsx
+++ b/alignments/reports/pseudReports_blastBasedAlignments_2021_Jan13.xlsx
@@ -1677,7 +1677,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -1737,7 +1737,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -1757,7 +1757,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -5773,31 +5773,61 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -5823,11 +5853,21 @@
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">

</xml_diff>